<commit_message>
cập nhật mới nhất
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,22 +486,22 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Thai Sản</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Việc Riêng</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Hiếu Hỉ</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Phép Năm</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Thai Sản</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Việc Riêng</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -517,7 +517,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>622204064</v>
+        <v>621605001</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
@@ -527,22 +527,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>HẢI</t>
+          <t>DŨNG</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>LÊ VIẾT</t>
+          <t>TRƯƠNG VĂN</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2018-08-01</t>
+          <t>08/01/2016</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NV PT Phần Mềm BP CNTT</t>
+          <t>TN Quản Trị Mạng BP CNTT</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -563,7 +563,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>622210012</v>
+        <v>622204064</v>
       </c>
       <c r="B3" t="n">
         <v>3</v>
@@ -573,17 +573,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SƠN</t>
+          <t>HẢI</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NGÔ QUỐC</t>
+          <t>LÊ VIẾT</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2020-08-01</t>
+          <t>08/01/2018</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -596,26 +596,168 @@
           <t>CNTT</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>40</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
+        <v>9</v>
+      </c>
+      <c r="K3" t="n">
         <v>10</v>
       </c>
-      <c r="K3" t="n">
-        <v>3</v>
-      </c>
       <c r="L3" t="n">
-        <v>8</v>
-      </c>
-      <c r="M3" t="n">
-        <v>2</v>
-      </c>
-      <c r="N3" t="n">
-        <v>16</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>622210012</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>SƠN</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NGÔ QUỐC</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>08/01/2020</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>NV PT Phần Mềm BP CNTT</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>CNTT</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>40</v>
+      </c>
+      <c r="J4" t="n">
+        <v>10</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>18</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>621805013</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NGHĨA</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ĐOÀN TRỌNG</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>05/18/2018</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>NV Hành chính BP HCNS</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>HCNS</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>621412001</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ý</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>PHAN NHƯ</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12/15/2014</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>NV CS Tiền lương BP HCNS</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>HCNS</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>